<commit_message>
Add error cases for PV tests
</commit_message>
<xml_diff>
--- a/tests/fixtures/npv.xlsx
+++ b/tests/fixtures/npv.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strauch\Documents\src\pycel\tests\fixtures\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7025A9-D98E-42BE-9B41-192406C3EBA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86EE158-CFF0-4DEF-A6B0-DFCB861A8418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="1815" windowWidth="34425" windowHeight="18270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="2010" windowWidth="18780" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NPV" sheetId="1" r:id="rId1"/>

</xml_diff>